<commit_message>
Firmen Aufgabe + Text
</commit_message>
<xml_diff>
--- a/GVI & WUB/GVI LF1/Gewinn & Verlustverteilung/Marie_GewinnVerlustAufteilung.xlsx
+++ b/GVI & WUB/GVI LF1/Gewinn & Verlustverteilung/Marie_GewinnVerlustAufteilung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dstemmler\Dokumente\GitHub\Danger_Gang_GVI\GVI &amp; WUB\GVI LF1\Gewinn &amp; Verlustverteilung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE855FD9-775A-427A-9417-21366F0D2E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF37B114-3A6F-48B3-A024-DC86FAA19499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{D92D6955-6253-487E-896C-0F947CDCEADE}"/>
   </bookViews>
@@ -475,18 +475,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C9A33F-FB13-449C-9EB9-8C295A3B304A}">
-  <dimension ref="D12:I44"/>
+  <dimension ref="A12:XFD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="D12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="5" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.68359375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1015625" customWidth="1"/>
+    <col min="5" max="5" width="18.41796875" customWidth="1"/>
+    <col min="6" max="6" width="10.9453125" customWidth="1"/>
+    <col min="7" max="7" width="13.7890625" customWidth="1"/>
+    <col min="8" max="8" width="20.3125" customWidth="1"/>
+    <col min="9" max="9" width="24.89453125" customWidth="1"/>
+    <col min="10" max="16383" width="10.9453125" hidden="1"/>
+    <col min="16384" max="16384" width="15" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="12" spans="4:9" x14ac:dyDescent="0.55000000000000004">
@@ -599,6 +604,7 @@
         <v>145596</v>
       </c>
     </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
     <row r="18" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" t="s">
         <v>4</v>
@@ -706,6 +712,10 @@
         <v>105596</v>
       </c>
     </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
     <row r="27" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -820,6 +830,7 @@
         <v>34000</v>
       </c>
     </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
     <row r="33" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" t="s">
         <v>4</v>
@@ -931,6 +942,9 @@
         <v>6000</v>
       </c>
     </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.55000000000000004"/>
     <row r="41" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="F41" t="s">
         <v>16</v>
@@ -979,8 +993,13 @@
         <v>1.3933010087499302</v>
       </c>
     </row>
+    <row r="45" spans="4:9" ht="9.3000000000000007" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;CGewinn Verlustaufteilung
+</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>